<commit_message>
update User_stories 19:27 09/04/2025
</commit_message>
<xml_diff>
--- a/Docs/User Story/User_Stories.xlsx
+++ b/Docs/User Story/User_Stories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Desktop\Project\Nyakko.EduConnect.Platform\Docs\User Story\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A716F7DB-6BE9-45B2-925D-70A4C4E1DFB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424FD5EE-1F4D-4273-B314-BBDA1F2F43FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'User Stories'!$C$2:$C$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'User Stories'!$C$2:$C$17</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="68">
   <si>
     <t>ID</t>
   </si>
@@ -390,6 +390,36 @@
   </si>
   <si>
     <t>Là một user, tôi có thể báo cáo (report) một người dùng khác nếu họ spam tin nhắn, spam nội dung hoặc đánh giá ảo,... để giúp duy trì môi trường sử dụng văn minh và an toàn.</t>
+  </si>
+  <si>
+    <t>US24</t>
+  </si>
+  <si>
+    <t>US25</t>
+  </si>
+  <si>
+    <t>US26</t>
+  </si>
+  <si>
+    <t>US27</t>
+  </si>
+  <si>
+    <t>US28</t>
+  </si>
+  <si>
+    <t>US29</t>
+  </si>
+  <si>
+    <t>US30</t>
+  </si>
+  <si>
+    <t>Là một user, tôi muốn xem danh sách các mục đã lưu (trường đại học, vị trí thực tập, bài viết, v.v.) để dễ dàng truy cập lại và tìm hiểu thêm khi cần.</t>
+  </si>
+  <si>
+    <t>Publisher</t>
+  </si>
+  <si>
+    <t>Là một Publisher, tôi có thể xem các form dữ liệu mà người dùng đã gửi đến cho tôi (ví dụ: đăng ký thực tập, đăng ký tư vấn nhập học...) để xử lý và phản hồi kịp thời.</t>
   </si>
 </sst>
 </file>
@@ -893,10 +923,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH109"/>
+  <dimension ref="A1:AH110"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1566,7 +1596,7 @@
         <v>16</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>32</v>
@@ -1604,7 +1634,7 @@
         <v>16</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>32</v>
@@ -1642,7 +1672,7 @@
         <v>16</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>32</v>
@@ -1680,7 +1710,7 @@
         <v>16</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>32</v>
@@ -1718,7 +1748,7 @@
         <v>16</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>32</v>
@@ -1794,7 +1824,7 @@
         <v>16</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>32</v>
@@ -1821,7 +1851,7 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:26" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>50</v>
       </c>
@@ -1832,7 +1862,7 @@
         <v>16</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>32</v>
@@ -1859,7 +1889,7 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
     </row>
-    <row r="24" spans="1:26" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>51</v>
       </c>
@@ -1870,7 +1900,7 @@
         <v>16</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>32</v>
@@ -1898,11 +1928,21 @@
       <c r="Z24" s="1"/>
     </row>
     <row r="25" spans="1:26" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="4"/>
+      <c r="A25" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
@@ -1926,11 +1966,21 @@
       <c r="Z25" s="1"/>
     </row>
     <row r="26" spans="1:26" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="4"/>
+      <c r="A26" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
@@ -1954,7 +2004,9 @@
       <c r="Z26" s="1"/>
     </row>
     <row r="27" spans="1:26" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="4"/>
+      <c r="A27" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="5"/>
@@ -1982,7 +2034,9 @@
       <c r="Z27" s="1"/>
     </row>
     <row r="28" spans="1:26" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="4"/>
+      <c r="A28" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="5"/>
@@ -2010,7 +2064,9 @@
       <c r="Z28" s="1"/>
     </row>
     <row r="29" spans="1:26" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="4"/>
+      <c r="A29" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="5"/>
@@ -2038,7 +2094,9 @@
       <c r="Z29" s="1"/>
     </row>
     <row r="30" spans="1:26" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="4"/>
+      <c r="A30" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="5"/>
@@ -2066,13 +2124,15 @@
       <c r="Z30" s="1"/>
     </row>
     <row r="31" spans="1:26" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="2"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="11"/>
+      <c r="A31" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="4"/>
       <c r="F31" s="1"/>
-      <c r="G31" s="11"/>
+      <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
@@ -2238,7 +2298,7 @@
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
-      <c r="E37" s="2"/>
+      <c r="E37" s="11"/>
       <c r="F37" s="1"/>
       <c r="G37" s="11"/>
       <c r="H37" s="1"/>
@@ -4277,24 +4337,52 @@
       <c r="Y109" s="1"/>
       <c r="Z109" s="1"/>
     </row>
+    <row r="110" spans="1:26" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="2"/>
+      <c r="B110" s="1"/>
+      <c r="C110" s="1"/>
+      <c r="D110" s="1"/>
+      <c r="E110" s="2"/>
+      <c r="F110" s="1"/>
+      <c r="G110" s="11"/>
+      <c r="H110" s="1"/>
+      <c r="I110" s="1"/>
+      <c r="J110" s="1"/>
+      <c r="K110" s="1"/>
+      <c r="L110" s="1"/>
+      <c r="M110" s="1"/>
+      <c r="N110" s="1"/>
+      <c r="O110" s="1"/>
+      <c r="P110" s="1"/>
+      <c r="Q110" s="1"/>
+      <c r="R110" s="1"/>
+      <c r="S110" s="1"/>
+      <c r="T110" s="1"/>
+      <c r="U110" s="1"/>
+      <c r="V110" s="1"/>
+      <c r="W110" s="1"/>
+      <c r="X110" s="1"/>
+      <c r="Y110" s="1"/>
+      <c r="Z110" s="1"/>
+    </row>
   </sheetData>
-  <autoFilter ref="C2:C16" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="C2:C17" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="1">
     <mergeCell ref="G2:G8"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C31:C109" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C32:C110" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Admin,User,New User"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z21:Z30 AA10:AA109" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z22:Z31 AA10:AA110" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"To Do,In Progress,Review,Blocked,Done,Cancelled"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Status Error" error="Invalid status!" promptTitle="Progress Status" prompt="Chọn trạng thái công việc" sqref="E37:E109 E2:E30" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Status Error" error="Invalid status!" promptTitle="Progress Status" prompt="Chọn trạng thái công việc" sqref="E38:E110 E2:E31" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"To Do,In Progress,Review,Blocked,Done,Cancelled"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C30" xr:uid="{68AAA0C7-2104-40A0-AEA8-79CA7503BDFA}">
-      <formula1>"Admin,Contributor,School Publisher,Internship Publisher,User,New User"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C31" xr:uid="{68AAA0C7-2104-40A0-AEA8-79CA7503BDFA}">
+      <formula1>"Admin,Moderator,Publisher,School Publisher,Internship Publisher,User,New User"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
update 10/04/2025 dd/mm/yyyy 4:08PM GMT+7
</commit_message>
<xml_diff>
--- a/Docs/User Story/User_Stories.xlsx
+++ b/Docs/User Story/User_Stories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Desktop\Project\Nyakko.EduConnect.Platform\Docs\User Story\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA9F94F5-C205-4DB4-A28F-816F89D9A625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC9652D9-240B-4D9E-ABD4-E029E04485BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'User Stories'!$C$2:$C$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'User Stories'!$E$1:$E$110</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -978,7 +978,7 @@
   <dimension ref="A1:AH110"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4420,7 +4420,6 @@
       <c r="Z110" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="C2:C17" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="1">
     <mergeCell ref="G2:G8"/>
   </mergeCells>

</xml_diff>